<commit_message>
added leave schema to this project
</commit_message>
<xml_diff>
--- a/client/TimeTable/CSE_4_subject_teachers.xlsx
+++ b/client/TimeTable/CSE_4_subject_teachers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Teacher</t>
   </si>
@@ -24,10 +24,61 @@
     <t>Subject</t>
   </si>
   <si>
-    <t>Arzoo pandey</t>
-  </si>
-  <si>
     <t>OOPS</t>
+  </si>
+  <si>
+    <t>Prakhar Golchha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSA </t>
+  </si>
+  <si>
+    <t>A.K shrivastav</t>
+  </si>
+  <si>
+    <t>DAA</t>
+  </si>
+  <si>
+    <t>Akash Sonkar</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>Devika Sahu</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>Diwan</t>
+  </si>
+  <si>
+    <t>CSA LAB</t>
+  </si>
+  <si>
+    <t>OOPS LAB</t>
+  </si>
+  <si>
+    <t>OPPS LAB</t>
+  </si>
+  <si>
+    <t>DBMS LAB</t>
+  </si>
+  <si>
+    <t>VL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anjum khan </t>
+  </si>
+  <si>
+    <t>Suyash Sahu</t>
+  </si>
+  <si>
+    <t>Palak Lunia</t>
+  </si>
+  <si>
+    <t>Ruchi Agrawal</t>
   </si>
 </sst>
 </file>
@@ -359,16 +410,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -381,10 +432,106 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>